<commit_message>
Zeitmitschrift + Gantt update
</commit_message>
<xml_diff>
--- a/Zeitmitschrift_learnhub.xlsx
+++ b/Zeitmitschrift_learnhub.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\learnHub\LearnHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D52EC802-B97B-4313-A0EB-00C92DAF39B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1857BCA7-2879-43B4-BAF8-4959ABA667B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -149,10 +149,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -469,22 +469,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AL8"/>
+  <dimension ref="A1:AN8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="92" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AE1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AM10" sqref="AM10"/>
+      <pane xSplit="1" topLeftCell="V1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AL29" sqref="AL29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="35" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="13.109375" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="35" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="16.7109375" customWidth="1"/>
+    <col min="37" max="37" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="38" max="39" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -596,11 +597,17 @@
       <c r="AK1" s="9">
         <v>45456</v>
       </c>
-      <c r="AL1" s="9" t="s">
+      <c r="AL1" s="9">
+        <v>45457</v>
+      </c>
+      <c r="AM1" s="9">
+        <v>45459</v>
+      </c>
+      <c r="AN1" s="9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:38" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:40" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -674,12 +681,14 @@
       <c r="AK2" s="8">
         <v>2</v>
       </c>
-      <c r="AL2" s="8">
+      <c r="AL2" s="8"/>
+      <c r="AM2" s="8"/>
+      <c r="AN2" s="8">
         <f>AI2+AC2+AB2+AA2+Z2+X2+W2+T2+S2+R2+M2+K2+G2+E2+C2+B2+AK2</f>
         <v>23.58</v>
       </c>
     </row>
-    <row r="3" spans="1:38" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:40" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -760,11 +769,15 @@
         <v>2</v>
       </c>
       <c r="AL3" s="8">
-        <f>AJ3+AI3+AH3+AG3+AF3+AE3+AB3+AA3+Z3+Y3+X3+W3+V3+U3+T3+R3+O3+M3+L3+AK3</f>
-        <v>33</v>
+        <v>0.5</v>
+      </c>
+      <c r="AM3" s="8"/>
+      <c r="AN3" s="8">
+        <f>AJ3+AI3+AH3+AG3+AF3+AE3+AB3+AA3+Z3+Y3+X3+W3+V3+U3+T3+R3+O3+M3+L3+AK3+AL3</f>
+        <v>33.5</v>
       </c>
     </row>
-    <row r="4" spans="1:38" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:40" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
@@ -849,11 +862,17 @@
         <v>2</v>
       </c>
       <c r="AL4" s="8">
-        <f>AI4+AH4+AG4+AF4+AE4+AD4+AC4+AB4+AA4+W4+T4+R4+Q4+P4+M4+L4+K4+F4+D4+B4+AK4</f>
-        <v>26.58</v>
+        <v>0.5</v>
+      </c>
+      <c r="AM4" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="AN4" s="8">
+        <f>AI4+AH4+AG4+AF4+AE4+AD4+AC4+AB4+AA4+W4+T4+R4+Q4+P4+M4+L4+K4+F4+D4+B4+AK4+AL4+AM4</f>
+        <v>27.33</v>
       </c>
     </row>
-    <row r="5" spans="1:38" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:40" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
@@ -926,11 +945,17 @@
         <v>2</v>
       </c>
       <c r="AL5" s="8">
-        <f>AJ5+AI5+AB5+AA5+Y5+X5+W5+R5+N5+M5+K5+J5+I5+H5+B5+AK5</f>
-        <v>24.25</v>
+        <v>0.5</v>
+      </c>
+      <c r="AM5" s="8">
+        <v>2</v>
+      </c>
+      <c r="AN5" s="8">
+        <f>AJ5+AI5+AB5+AA5+Y5+X5+W5+R5+N5+M5+K5+J5+I5+H5+B5+AK5+AL5+AM5</f>
+        <v>26.75</v>
       </c>
     </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.3">
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
@@ -967,8 +992,10 @@
       <c r="AI6" s="7"/>
       <c r="AJ6" s="7"/>
       <c r="AK6" s="7"/>
+      <c r="AL6" s="7"/>
+      <c r="AM6" s="7"/>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.3">
       <c r="B8" s="7"/>
     </row>
   </sheetData>

</xml_diff>